<commit_message>
Class formulation for Plotting Lineup
</commit_message>
<xml_diff>
--- a/Data/2024/Lineup/Results.xlsx
+++ b/Data/2024/Lineup/Results.xlsx
@@ -825,6 +825,9 @@
       <c r="N2" s="4">
         <v>7</v>
       </c>
+      <c r="O2" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="3" t="s">
@@ -869,6 +872,9 @@
       <c r="N3" s="4">
         <v>-19</v>
       </c>
+      <c r="O3" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="5" t="s">
@@ -913,6 +919,9 @@
       <c r="N4" s="4">
         <v>9</v>
       </c>
+      <c r="O4" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="5" t="s">
@@ -957,6 +966,9 @@
       <c r="N5" s="4">
         <v>4</v>
       </c>
+      <c r="O5" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="6" t="s">
@@ -1001,6 +1013,9 @@
       <c r="N6" s="4">
         <v>20</v>
       </c>
+      <c r="O6" s="4">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="6" t="s">
@@ -1045,6 +1060,9 @@
       <c r="N7" s="4">
         <v>17</v>
       </c>
+      <c r="O7" s="4">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="6" t="s">
@@ -1089,6 +1107,9 @@
       <c r="N8" s="4">
         <v>0</v>
       </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="7" t="s">
@@ -1133,6 +1154,9 @@
       <c r="N9" s="4">
         <v>7</v>
       </c>
+      <c r="O9" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="7" t="s">
@@ -1177,6 +1201,9 @@
       <c r="N10" s="4">
         <v>0</v>
       </c>
+      <c r="O10" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="8" t="s">
@@ -1221,6 +1248,9 @@
       <c r="N11" s="4">
         <v>1</v>
       </c>
+      <c r="O11" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="8" t="s">
@@ -1265,6 +1295,9 @@
       <c r="N12" s="4">
         <v>0</v>
       </c>
+      <c r="O12" s="4">
+        <v>-18</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="9" t="s">
@@ -1309,6 +1342,9 @@
       <c r="N13" s="4">
         <v>28</v>
       </c>
+      <c r="O13" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="9" t="s">
@@ -1353,6 +1389,9 @@
       <c r="N14" s="4">
         <v>46</v>
       </c>
+      <c r="O14" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="10" t="s">
@@ -1397,6 +1436,9 @@
       <c r="N15" s="4">
         <v>26</v>
       </c>
+      <c r="O15" s="4">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="10" t="s">
@@ -1441,6 +1483,9 @@
       <c r="N16" s="4">
         <v>27</v>
       </c>
+      <c r="O16" s="4">
+        <v>-21</v>
+      </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="11" t="s">
@@ -1485,6 +1530,9 @@
       <c r="N17" s="4">
         <v>4</v>
       </c>
+      <c r="O17" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="11" t="s">
@@ -1529,6 +1577,9 @@
       <c r="N18" s="4">
         <v>1</v>
       </c>
+      <c r="O18" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="12" t="s">
@@ -1573,6 +1624,9 @@
       <c r="N19" s="4">
         <v>17</v>
       </c>
+      <c r="O19" s="4">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="12" t="s">
@@ -1617,6 +1671,9 @@
       <c r="N20" s="4">
         <v>20</v>
       </c>
+      <c r="O20" s="4">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="13" t="s">
@@ -1661,6 +1718,9 @@
       <c r="N21" s="4">
         <v>5</v>
       </c>
+      <c r="O21" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="13" t="s">
@@ -1705,6 +1765,9 @@
       <c r="N22" s="4">
         <v>1</v>
       </c>
+      <c r="O22" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="1" t="s">
@@ -1826,6 +1889,9 @@
       <c r="N25" s="4">
         <v>10.5</v>
       </c>
+      <c r="O25" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="3" t="s">
@@ -1870,6 +1936,9 @@
       <c r="N26" s="4">
         <v>9.9</v>
       </c>
+      <c r="O26" s="4">
+        <v>9.699999999999999</v>
+      </c>
     </row>
     <row r="27" spans="1:25">
       <c r="A27" s="5" t="s">
@@ -1914,6 +1983,9 @@
       <c r="N27" s="4">
         <v>15.1</v>
       </c>
+      <c r="O27" s="4">
+        <v>15.2</v>
+      </c>
     </row>
     <row r="28" spans="1:25">
       <c r="A28" s="5" t="s">
@@ -1958,6 +2030,9 @@
       <c r="N28" s="4">
         <v>16.6</v>
       </c>
+      <c r="O28" s="4">
+        <v>16.3</v>
+      </c>
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="6" t="s">
@@ -2002,6 +2077,9 @@
       <c r="N29" s="4">
         <v>23</v>
       </c>
+      <c r="O29" s="4">
+        <v>23.3</v>
+      </c>
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="6" t="s">
@@ -2046,6 +2124,9 @@
       <c r="N30" s="4">
         <v>22.2</v>
       </c>
+      <c r="O30" s="4">
+        <v>22.5</v>
+      </c>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="6" t="s">
@@ -2090,6 +2171,9 @@
       <c r="N31" s="4">
         <v>0</v>
       </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="7" t="s">
@@ -2134,6 +2218,9 @@
       <c r="N32" s="4">
         <v>10.8</v>
       </c>
+      <c r="O32" s="4">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="7" t="s">
@@ -2178,6 +2265,9 @@
       <c r="N33" s="4">
         <v>9.699999999999999</v>
       </c>
+      <c r="O33" s="4">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="8" t="s">
@@ -2222,6 +2312,9 @@
       <c r="N34" s="4">
         <v>7.7</v>
       </c>
+      <c r="O34" s="4">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="8" t="s">
@@ -2266,6 +2359,9 @@
       <c r="N35" s="4">
         <v>7.5</v>
       </c>
+      <c r="O35" s="4">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="36" spans="1:25">
       <c r="A36" s="9" t="s">
@@ -2310,6 +2406,9 @@
       <c r="N36" s="4">
         <v>26.1</v>
       </c>
+      <c r="O36" s="4">
+        <v>26.2</v>
+      </c>
     </row>
     <row r="37" spans="1:25">
       <c r="A37" s="9" t="s">
@@ -2354,6 +2453,9 @@
       <c r="N37" s="4">
         <v>22.3</v>
       </c>
+      <c r="O37" s="4">
+        <v>23.3</v>
+      </c>
     </row>
     <row r="38" spans="1:25">
       <c r="A38" s="10" t="s">
@@ -2398,6 +2500,9 @@
       <c r="N38" s="4">
         <v>22.8</v>
       </c>
+      <c r="O38" s="4">
+        <v>23.1</v>
+      </c>
     </row>
     <row r="39" spans="1:25">
       <c r="A39" s="10" t="s">
@@ -2442,6 +2547,9 @@
       <c r="N39" s="4">
         <v>20.9</v>
       </c>
+      <c r="O39" s="4">
+        <v>21.2</v>
+      </c>
     </row>
     <row r="40" spans="1:25">
       <c r="A40" s="11" t="s">
@@ -2486,6 +2594,9 @@
       <c r="N40" s="4">
         <v>10.5</v>
       </c>
+      <c r="O40" s="4">
+        <v>10.4</v>
+      </c>
     </row>
     <row r="41" spans="1:25">
       <c r="A41" s="11" t="s">
@@ -2530,6 +2641,9 @@
       <c r="N41" s="4">
         <v>10.9</v>
       </c>
+      <c r="O41" s="4">
+        <v>10.8</v>
+      </c>
     </row>
     <row r="42" spans="1:25">
       <c r="A42" s="12" t="s">
@@ -2574,6 +2688,9 @@
       <c r="N42" s="4">
         <v>31</v>
       </c>
+      <c r="O42" s="4">
+        <v>31.1</v>
+      </c>
     </row>
     <row r="43" spans="1:25">
       <c r="A43" s="12" t="s">
@@ -2618,6 +2735,9 @@
       <c r="N43" s="4">
         <v>22.7</v>
       </c>
+      <c r="O43" s="4">
+        <v>23</v>
+      </c>
     </row>
     <row r="44" spans="1:25">
       <c r="A44" s="13" t="s">
@@ -2662,6 +2782,9 @@
       <c r="N44" s="4">
         <v>9</v>
       </c>
+      <c r="O44" s="4">
+        <v>8.9</v>
+      </c>
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="13" t="s">
@@ -2706,6 +2829,9 @@
       <c r="N45" s="4">
         <v>5.2</v>
       </c>
+      <c r="O45" s="4">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="47" spans="1:25">
       <c r="A47" s="1" t="s">
@@ -2827,8 +2953,11 @@
       <c r="N48" s="4">
         <v>62</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="O48" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="3" t="s">
         <v>26</v>
       </c>
@@ -2871,8 +3000,11 @@
       <c r="N49" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="O49" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="5" t="s">
         <v>27</v>
       </c>
@@ -2915,8 +3047,11 @@
       <c r="N50" s="4">
         <v>81</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="O50" s="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="5" t="s">
         <v>28</v>
       </c>
@@ -2959,8 +3094,11 @@
       <c r="N51" s="4">
         <v>115</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="O51" s="4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="6" t="s">
         <v>29</v>
       </c>
@@ -3003,8 +3141,11 @@
       <c r="N52" s="4">
         <v>304</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="O52" s="4">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="6" t="s">
         <v>30</v>
       </c>
@@ -3047,8 +3188,11 @@
       <c r="N53" s="4">
         <v>279</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="O53" s="4">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="7" t="s">
         <v>32</v>
       </c>
@@ -3091,8 +3235,11 @@
       <c r="N54" s="4">
         <v>81</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="O54" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="7" t="s">
         <v>33</v>
       </c>
@@ -3135,8 +3282,11 @@
       <c r="N55" s="4">
         <v>74</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="O55" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="8" t="s">
         <v>34</v>
       </c>
@@ -3179,8 +3329,11 @@
       <c r="N56" s="4">
         <v>33</v>
       </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="O56" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="8" t="s">
         <v>35</v>
       </c>
@@ -3223,8 +3376,11 @@
       <c r="N57" s="4">
         <v>46</v>
       </c>
-    </row>
-    <row r="58" spans="1:14">
+      <c r="O57" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="9" t="s">
         <v>36</v>
       </c>
@@ -3267,8 +3423,11 @@
       <c r="N58" s="4">
         <v>341</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="O58" s="4">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="9" t="s">
         <v>37</v>
       </c>
@@ -3311,8 +3470,11 @@
       <c r="N59" s="4">
         <v>292</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="O59" s="4">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="10" t="s">
         <v>38</v>
       </c>
@@ -3355,8 +3517,11 @@
       <c r="N60" s="4">
         <v>247</v>
       </c>
-    </row>
-    <row r="61" spans="1:14">
+      <c r="O60" s="4">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="10" t="s">
         <v>39</v>
       </c>
@@ -3399,8 +3564,11 @@
       <c r="N61" s="4">
         <v>236</v>
       </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="O61" s="4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="11" t="s">
         <v>40</v>
       </c>
@@ -3443,8 +3611,11 @@
       <c r="N62" s="4">
         <v>72</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="O62" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="11" t="s">
         <v>41</v>
       </c>
@@ -3487,8 +3658,11 @@
       <c r="N63" s="4">
         <v>32</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="O63" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="12" t="s">
         <v>42</v>
       </c>
@@ -3530,6 +3704,9 @@
       </c>
       <c r="N64" s="4">
         <v>410</v>
+      </c>
+      <c r="O64" s="4">
+        <v>445</v>
       </c>
     </row>
     <row r="65" spans="1:25">
@@ -3575,6 +3752,9 @@
       <c r="N65" s="4">
         <v>224</v>
       </c>
+      <c r="O65" s="4">
+        <v>243</v>
+      </c>
     </row>
     <row r="66" spans="1:25">
       <c r="A66" s="13" t="s">
@@ -3619,6 +3799,9 @@
       <c r="N66" s="4">
         <v>11</v>
       </c>
+      <c r="O66" s="4">
+        <v>13</v>
+      </c>
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="13" t="s">
@@ -3663,6 +3846,9 @@
       <c r="N67" s="4">
         <v>6</v>
       </c>
+      <c r="O67" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="68" spans="1:25">
       <c r="A68" s="6" t="s">
@@ -3707,6 +3893,9 @@
       <c r="N68" s="4">
         <v>26</v>
       </c>
+      <c r="O68" s="4">
+        <v>26</v>
+      </c>
     </row>
     <row r="70" spans="1:25">
       <c r="A70" s="1" t="s">
@@ -3828,6 +4017,9 @@
       <c r="N71" s="4">
         <v>119.8</v>
       </c>
+      <c r="O71" s="4">
+        <v>130.8</v>
+      </c>
     </row>
     <row r="72" spans="1:25">
       <c r="A72" s="3" t="s">
@@ -3872,6 +4064,9 @@
       <c r="N72" s="4">
         <v>109.2</v>
       </c>
+      <c r="O72" s="4">
+        <v>118.9</v>
+      </c>
     </row>
     <row r="73" spans="1:25">
       <c r="A73" s="5" t="s">
@@ -3916,6 +4111,9 @@
       <c r="N73" s="4">
         <v>167.7</v>
       </c>
+      <c r="O73" s="4">
+        <v>182.9</v>
+      </c>
     </row>
     <row r="74" spans="1:25">
       <c r="A74" s="5" t="s">
@@ -3960,6 +4158,9 @@
       <c r="N74" s="4">
         <v>212.6</v>
       </c>
+      <c r="O74" s="4">
+        <v>228.9</v>
+      </c>
     </row>
     <row r="75" spans="1:25">
       <c r="A75" s="6" t="s">
@@ -4004,6 +4205,9 @@
       <c r="N75" s="4">
         <v>285.1</v>
       </c>
+      <c r="O75" s="4">
+        <v>308.4</v>
+      </c>
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="6" t="s">
@@ -4048,6 +4252,9 @@
       <c r="N76" s="4">
         <v>249.1</v>
       </c>
+      <c r="O76" s="4">
+        <v>271.6</v>
+      </c>
     </row>
     <row r="77" spans="1:25">
       <c r="A77" s="7" t="s">
@@ -4092,6 +4299,9 @@
       <c r="N77" s="4">
         <v>112.8</v>
       </c>
+      <c r="O77" s="4">
+        <v>124.1</v>
+      </c>
     </row>
     <row r="78" spans="1:25">
       <c r="A78" s="7" t="s">
@@ -4136,6 +4346,9 @@
       <c r="N78" s="4">
         <v>102</v>
       </c>
+      <c r="O78" s="4">
+        <v>111.5</v>
+      </c>
     </row>
     <row r="79" spans="1:25">
       <c r="A79" s="8" t="s">
@@ -4180,6 +4393,9 @@
       <c r="N79" s="4">
         <v>89.20000000000002</v>
       </c>
+      <c r="O79" s="4">
+        <v>96.80000000000001</v>
+      </c>
     </row>
     <row r="80" spans="1:25">
       <c r="A80" s="8" t="s">
@@ -4224,6 +4440,9 @@
       <c r="N80" s="4">
         <v>94.5</v>
       </c>
+      <c r="O80" s="4">
+        <v>101.8</v>
+      </c>
     </row>
     <row r="81" spans="1:25">
       <c r="A81" s="9" t="s">
@@ -4268,6 +4487,9 @@
       <c r="N81" s="4">
         <v>320</v>
       </c>
+      <c r="O81" s="4">
+        <v>346.2</v>
+      </c>
     </row>
     <row r="82" spans="1:25">
       <c r="A82" s="9" t="s">
@@ -4312,6 +4534,9 @@
       <c r="N82" s="4">
         <v>266.4</v>
       </c>
+      <c r="O82" s="4">
+        <v>289.7</v>
+      </c>
     </row>
     <row r="83" spans="1:25">
       <c r="A83" s="10" t="s">
@@ -4356,6 +4581,9 @@
       <c r="N83" s="4">
         <v>260.5</v>
       </c>
+      <c r="O83" s="4">
+        <v>283.6</v>
+      </c>
     </row>
     <row r="84" spans="1:25">
       <c r="A84" s="10" t="s">
@@ -4400,6 +4628,9 @@
       <c r="N84" s="4">
         <v>257.1</v>
       </c>
+      <c r="O84" s="4">
+        <v>278.3</v>
+      </c>
     </row>
     <row r="85" spans="1:25">
       <c r="A85" s="11" t="s">
@@ -4444,6 +4675,9 @@
       <c r="N85" s="4">
         <v>116.6</v>
       </c>
+      <c r="O85" s="4">
+        <v>127</v>
+      </c>
     </row>
     <row r="86" spans="1:25">
       <c r="A86" s="11" t="s">
@@ -4488,6 +4722,9 @@
       <c r="N86" s="4">
         <v>121.7</v>
       </c>
+      <c r="O86" s="4">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="87" spans="1:25">
       <c r="A87" s="12" t="s">
@@ -4532,6 +4769,9 @@
       <c r="N87" s="4">
         <v>394.8</v>
       </c>
+      <c r="O87" s="4">
+        <v>425.9</v>
+      </c>
     </row>
     <row r="88" spans="1:25">
       <c r="A88" s="12" t="s">
@@ -4576,6 +4816,9 @@
       <c r="N88" s="4">
         <v>292.1</v>
       </c>
+      <c r="O88" s="4">
+        <v>315.1</v>
+      </c>
     </row>
     <row r="89" spans="1:25">
       <c r="A89" s="13" t="s">
@@ -4620,6 +4863,9 @@
       <c r="N89" s="4">
         <v>100.7</v>
       </c>
+      <c r="O89" s="4">
+        <v>109.6</v>
+      </c>
     </row>
     <row r="90" spans="1:25">
       <c r="A90" s="13" t="s">
@@ -4664,6 +4910,9 @@
       <c r="N90" s="4">
         <v>74.40000000000001</v>
       </c>
+      <c r="O90" s="4">
+        <v>79.5</v>
+      </c>
     </row>
     <row r="91" spans="1:25">
       <c r="A91" s="6" t="s">
@@ -4708,6 +4957,9 @@
       <c r="N91" s="4">
         <v>14</v>
       </c>
+      <c r="O91" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="93" spans="1:25">
       <c r="A93" s="1" t="s">
@@ -4829,6 +5081,9 @@
       <c r="N94" s="4">
         <v>4.769230769230769</v>
       </c>
+      <c r="O94" s="4">
+        <v>5.142857142857143</v>
+      </c>
     </row>
     <row r="95" spans="1:25">
       <c r="A95" s="3" t="s">
@@ -4873,6 +5128,9 @@
       <c r="N95" s="4">
         <v>1.615384615384615</v>
       </c>
+      <c r="O95" s="4">
+        <v>1.714285714285714</v>
+      </c>
     </row>
     <row r="96" spans="1:25">
       <c r="A96" s="5" t="s">
@@ -4917,8 +5175,11 @@
       <c r="N96" s="4">
         <v>6.230769230769231</v>
       </c>
-    </row>
-    <row r="97" spans="1:14">
+      <c r="O96" s="4">
+        <v>6.285714285714286</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97" s="5" t="s">
         <v>28</v>
       </c>
@@ -4961,8 +5222,11 @@
       <c r="N97" s="4">
         <v>8.846153846153847</v>
       </c>
-    </row>
-    <row r="98" spans="1:14">
+      <c r="O97" s="4">
+        <v>8.857142857142858</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" s="6" t="s">
         <v>29</v>
       </c>
@@ -5005,8 +5269,11 @@
       <c r="N98" s="4">
         <v>23.38461538461538</v>
       </c>
-    </row>
-    <row r="99" spans="1:14">
+      <c r="O98" s="4">
+        <v>23.28571428571428</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99" s="6" t="s">
         <v>30</v>
       </c>
@@ -5049,8 +5316,11 @@
       <c r="N99" s="4">
         <v>21.46153846153846</v>
       </c>
-    </row>
-    <row r="100" spans="1:14">
+      <c r="O99" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
       <c r="A100" s="7" t="s">
         <v>32</v>
       </c>
@@ -5093,8 +5363,11 @@
       <c r="N100" s="4">
         <v>6.230769230769231</v>
       </c>
-    </row>
-    <row r="101" spans="1:14">
+      <c r="O100" s="4">
+        <v>6.214285714285714</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
       <c r="A101" s="7" t="s">
         <v>33</v>
       </c>
@@ -5137,8 +5410,11 @@
       <c r="N101" s="4">
         <v>5.692307692307693</v>
       </c>
-    </row>
-    <row r="102" spans="1:14">
+      <c r="O101" s="4">
+        <v>5.428571428571429</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
       <c r="A102" s="8" t="s">
         <v>34</v>
       </c>
@@ -5181,8 +5457,11 @@
       <c r="N102" s="4">
         <v>2.538461538461538</v>
       </c>
-    </row>
-    <row r="103" spans="1:14">
+      <c r="O102" s="4">
+        <v>2.571428571428572</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
       <c r="A103" s="8" t="s">
         <v>35</v>
       </c>
@@ -5225,8 +5504,11 @@
       <c r="N103" s="4">
         <v>3.538461538461538</v>
       </c>
-    </row>
-    <row r="104" spans="1:14">
+      <c r="O103" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
       <c r="A104" s="9" t="s">
         <v>36</v>
       </c>
@@ -5269,8 +5551,11 @@
       <c r="N104" s="4">
         <v>26.23076923076923</v>
       </c>
-    </row>
-    <row r="105" spans="1:14">
+      <c r="O104" s="4">
+        <v>25.57142857142857</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
       <c r="A105" s="9" t="s">
         <v>37</v>
       </c>
@@ -5313,8 +5598,11 @@
       <c r="N105" s="4">
         <v>22.46153846153846</v>
       </c>
-    </row>
-    <row r="106" spans="1:14">
+      <c r="O105" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
       <c r="A106" s="10" t="s">
         <v>38</v>
       </c>
@@ -5357,8 +5645,11 @@
       <c r="N106" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:14">
+      <c r="O106" s="4">
+        <v>20.92857142857143</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
       <c r="A107" s="10" t="s">
         <v>39</v>
       </c>
@@ -5401,8 +5692,11 @@
       <c r="N107" s="4">
         <v>18.15384615384615</v>
       </c>
-    </row>
-    <row r="108" spans="1:14">
+      <c r="O107" s="4">
+        <v>15.35714285714286</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
       <c r="A108" s="11" t="s">
         <v>40</v>
       </c>
@@ -5445,8 +5739,11 @@
       <c r="N108" s="4">
         <v>5.538461538461538</v>
       </c>
-    </row>
-    <row r="109" spans="1:14">
+      <c r="O108" s="4">
+        <v>5.571428571428571</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15">
       <c r="A109" s="11" t="s">
         <v>41</v>
       </c>
@@ -5489,8 +5786,11 @@
       <c r="N109" s="4">
         <v>2.461538461538462</v>
       </c>
-    </row>
-    <row r="110" spans="1:14">
+      <c r="O109" s="4">
+        <v>2.857142857142857</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15">
       <c r="A110" s="12" t="s">
         <v>42</v>
       </c>
@@ -5533,8 +5833,11 @@
       <c r="N110" s="4">
         <v>31.53846153846154</v>
       </c>
-    </row>
-    <row r="111" spans="1:14">
+      <c r="O110" s="4">
+        <v>31.78571428571428</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
       <c r="A111" s="12" t="s">
         <v>43</v>
       </c>
@@ -5577,8 +5880,11 @@
       <c r="N111" s="4">
         <v>17.23076923076923</v>
       </c>
-    </row>
-    <row r="112" spans="1:14">
+      <c r="O111" s="4">
+        <v>17.35714285714286</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
       <c r="A112" s="13" t="s">
         <v>44</v>
       </c>
@@ -5620,6 +5926,9 @@
       </c>
       <c r="N112" s="4">
         <v>0.8461538461538461</v>
+      </c>
+      <c r="O112" s="4">
+        <v>0.9285714285714286</v>
       </c>
     </row>
     <row r="113" spans="1:25">
@@ -5665,6 +5974,9 @@
       <c r="N113" s="4">
         <v>0.4615384615384616</v>
       </c>
+      <c r="O113" s="4">
+        <v>0.5714285714285714</v>
+      </c>
     </row>
     <row r="114" spans="1:25">
       <c r="A114" s="6" t="s">
@@ -5709,6 +6021,9 @@
       <c r="N114" s="4">
         <v>2</v>
       </c>
+      <c r="O114" s="4">
+        <v>1.857142857142857</v>
+      </c>
     </row>
     <row r="116" spans="1:25">
       <c r="A116" s="1" t="s">
@@ -5830,6 +6145,9 @@
       <c r="N117" s="4">
         <v>9.215384615384615</v>
       </c>
+      <c r="O117" s="4">
+        <v>9.342857142857143</v>
+      </c>
     </row>
     <row r="118" spans="1:25">
       <c r="A118" s="3" t="s">
@@ -5874,6 +6192,9 @@
       <c r="N118" s="4">
         <v>8.399999999999999</v>
       </c>
+      <c r="O118" s="4">
+        <v>8.492857142857142</v>
+      </c>
     </row>
     <row r="119" spans="1:25">
       <c r="A119" s="5" t="s">
@@ -5918,6 +6239,9 @@
       <c r="N119" s="4">
         <v>12.9</v>
       </c>
+      <c r="O119" s="4">
+        <v>13.06428571428571</v>
+      </c>
     </row>
     <row r="120" spans="1:25">
       <c r="A120" s="5" t="s">
@@ -5962,6 +6286,9 @@
       <c r="N120" s="4">
         <v>16.35384615384615</v>
       </c>
+      <c r="O120" s="4">
+        <v>16.35</v>
+      </c>
     </row>
     <row r="121" spans="1:25">
       <c r="A121" s="6" t="s">
@@ -6006,6 +6333,9 @@
       <c r="N121" s="4">
         <v>21.93076923076923</v>
       </c>
+      <c r="O121" s="4">
+        <v>22.02857142857143</v>
+      </c>
     </row>
     <row r="122" spans="1:25">
       <c r="A122" s="6" t="s">
@@ -6050,6 +6380,9 @@
       <c r="N122" s="4">
         <v>19.16153846153846</v>
       </c>
+      <c r="O122" s="4">
+        <v>19.4</v>
+      </c>
     </row>
     <row r="123" spans="1:25">
       <c r="A123" s="7" t="s">
@@ -6094,6 +6427,9 @@
       <c r="N123" s="4">
         <v>8.676923076923078</v>
       </c>
+      <c r="O123" s="4">
+        <v>8.864285714285716</v>
+      </c>
     </row>
     <row r="124" spans="1:25">
       <c r="A124" s="7" t="s">
@@ -6138,6 +6474,9 @@
       <c r="N124" s="4">
         <v>7.846153846153848</v>
       </c>
+      <c r="O124" s="4">
+        <v>7.964285714285715</v>
+      </c>
     </row>
     <row r="125" spans="1:25">
       <c r="A125" s="8" t="s">
@@ -6182,6 +6521,9 @@
       <c r="N125" s="4">
         <v>6.861538461538463</v>
       </c>
+      <c r="O125" s="4">
+        <v>6.914285714285715</v>
+      </c>
     </row>
     <row r="126" spans="1:25">
       <c r="A126" s="8" t="s">
@@ -6226,6 +6568,9 @@
       <c r="N126" s="4">
         <v>7.269230769230769</v>
       </c>
+      <c r="O126" s="4">
+        <v>7.271428571428571</v>
+      </c>
     </row>
     <row r="127" spans="1:25">
       <c r="A127" s="9" t="s">
@@ -6270,6 +6615,9 @@
       <c r="N127" s="4">
         <v>24.61538461538462</v>
       </c>
+      <c r="O127" s="4">
+        <v>24.72857142857143</v>
+      </c>
     </row>
     <row r="128" spans="1:25">
       <c r="A128" s="9" t="s">
@@ -6314,6 +6662,9 @@
       <c r="N128" s="4">
         <v>20.49230769230769</v>
       </c>
+      <c r="O128" s="4">
+        <v>20.69285714285715</v>
+      </c>
     </row>
     <row r="129" spans="1:25">
       <c r="A129" s="10" t="s">
@@ -6358,6 +6709,9 @@
       <c r="N129" s="4">
         <v>20.03846153846154</v>
       </c>
+      <c r="O129" s="4">
+        <v>20.25714285714286</v>
+      </c>
     </row>
     <row r="130" spans="1:25">
       <c r="A130" s="10" t="s">
@@ -6402,6 +6756,9 @@
       <c r="N130" s="4">
         <v>19.77692307692308</v>
       </c>
+      <c r="O130" s="4">
+        <v>19.87857142857143</v>
+      </c>
     </row>
     <row r="131" spans="1:25">
       <c r="A131" s="11" t="s">
@@ -6446,6 +6803,9 @@
       <c r="N131" s="4">
         <v>8.969230769230769</v>
       </c>
+      <c r="O131" s="4">
+        <v>9.071428571428571</v>
+      </c>
     </row>
     <row r="132" spans="1:25">
       <c r="A132" s="11" t="s">
@@ -6490,6 +6850,9 @@
       <c r="N132" s="4">
         <v>9.361538461538462</v>
       </c>
+      <c r="O132" s="4">
+        <v>9.464285714285714</v>
+      </c>
     </row>
     <row r="133" spans="1:25">
       <c r="A133" s="12" t="s">
@@ -6534,6 +6897,9 @@
       <c r="N133" s="4">
         <v>30.36923076923076</v>
       </c>
+      <c r="O133" s="4">
+        <v>30.42142857142857</v>
+      </c>
     </row>
     <row r="134" spans="1:25">
       <c r="A134" s="12" t="s">
@@ -6578,6 +6944,9 @@
       <c r="N134" s="4">
         <v>22.46923076923077</v>
       </c>
+      <c r="O134" s="4">
+        <v>22.50714285714286</v>
+      </c>
     </row>
     <row r="135" spans="1:25">
       <c r="A135" s="13" t="s">
@@ -6622,6 +6991,9 @@
       <c r="N135" s="4">
         <v>7.746153846153845</v>
       </c>
+      <c r="O135" s="4">
+        <v>7.828571428571428</v>
+      </c>
     </row>
     <row r="136" spans="1:25">
       <c r="A136" s="13" t="s">
@@ -6666,6 +7038,9 @@
       <c r="N136" s="4">
         <v>5.723076923076923</v>
       </c>
+      <c r="O136" s="4">
+        <v>5.678571428571429</v>
+      </c>
     </row>
     <row r="137" spans="1:25">
       <c r="A137" s="6" t="s">
@@ -6710,6 +7085,9 @@
       <c r="N137" s="4">
         <v>1.076923076923077</v>
       </c>
+      <c r="O137" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:25">
       <c r="A139" s="1" t="s">
@@ -6831,6 +7209,9 @@
       <c r="N140" s="4">
         <v>0.6666666666666666</v>
       </c>
+      <c r="O140" s="4">
+        <v>0.9090909090909091</v>
+      </c>
     </row>
     <row r="141" spans="1:25">
       <c r="A141" s="3" t="s">
@@ -6875,6 +7256,9 @@
       <c r="N141" s="4">
         <v>-1.919191919191919</v>
       </c>
+      <c r="O141" s="4">
+        <v>0.3092783505154639</v>
+      </c>
     </row>
     <row r="142" spans="1:25">
       <c r="A142" s="5" t="s">
@@ -6919,6 +7303,9 @@
       <c r="N142" s="4">
         <v>0.5960264900662252</v>
       </c>
+      <c r="O142" s="4">
+        <v>0.4605263157894737</v>
+      </c>
     </row>
     <row r="143" spans="1:25">
       <c r="A143" s="5" t="s">
@@ -6963,6 +7350,9 @@
       <c r="N143" s="4">
         <v>0.2409638554216867</v>
       </c>
+      <c r="O143" s="4">
+        <v>0.5521472392638036</v>
+      </c>
     </row>
     <row r="144" spans="1:25">
       <c r="A144" s="6" t="s">
@@ -7007,8 +7397,11 @@
       <c r="N144" s="4">
         <v>0.8695652173913043</v>
       </c>
-    </row>
-    <row r="145" spans="1:14">
+      <c r="O144" s="4">
+        <v>0.944206008583691</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15">
       <c r="A145" s="6" t="s">
         <v>30</v>
       </c>
@@ -7051,8 +7444,11 @@
       <c r="N145" s="4">
         <v>0.7657657657657658</v>
       </c>
-    </row>
-    <row r="146" spans="1:14">
+      <c r="O145" s="4">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15">
       <c r="A146" s="7" t="s">
         <v>32</v>
       </c>
@@ -7095,8 +7491,11 @@
       <c r="N146" s="4">
         <v>0.6481481481481481</v>
       </c>
-    </row>
-    <row r="147" spans="1:14">
+      <c r="O146" s="4">
+        <v>0.5309734513274336</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15">
       <c r="A147" s="7" t="s">
         <v>33</v>
       </c>
@@ -7139,8 +7538,11 @@
       <c r="N147" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:14">
+      <c r="O147" s="4">
+        <v>0.2105263157894737</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15">
       <c r="A148" s="8" t="s">
         <v>34</v>
       </c>
@@ -7183,8 +7585,11 @@
       <c r="N148" s="4">
         <v>0.1298701298701299</v>
       </c>
-    </row>
-    <row r="149" spans="1:14">
+      <c r="O148" s="4">
+        <v>0.3947368421052632</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15">
       <c r="A149" s="8" t="s">
         <v>35</v>
       </c>
@@ -7227,8 +7632,11 @@
       <c r="N149" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:14">
+      <c r="O149" s="4">
+        <v>-2.465753424657534</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15">
       <c r="A150" s="9" t="s">
         <v>36</v>
       </c>
@@ -7271,8 +7679,11 @@
       <c r="N150" s="4">
         <v>1.0727969348659</v>
       </c>
-    </row>
-    <row r="151" spans="1:14">
+      <c r="O150" s="4">
+        <v>0.648854961832061</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15">
       <c r="A151" s="9" t="s">
         <v>37</v>
       </c>
@@ -7315,8 +7726,11 @@
       <c r="N151" s="4">
         <v>2.062780269058296</v>
       </c>
-    </row>
-    <row r="152" spans="1:14">
+      <c r="O151" s="4">
+        <v>1.28755364806867</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15">
       <c r="A152" s="10" t="s">
         <v>38</v>
       </c>
@@ -7359,8 +7773,11 @@
       <c r="N152" s="4">
         <v>1.140350877192982</v>
       </c>
-    </row>
-    <row r="153" spans="1:14">
+      <c r="O152" s="4">
+        <v>1.991341991341991</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15">
       <c r="A153" s="10" t="s">
         <v>39</v>
       </c>
@@ -7403,8 +7820,11 @@
       <c r="N153" s="4">
         <v>1.291866028708134</v>
       </c>
-    </row>
-    <row r="154" spans="1:14">
+      <c r="O153" s="4">
+        <v>-0.9905660377358491</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15">
       <c r="A154" s="11" t="s">
         <v>40</v>
       </c>
@@ -7447,8 +7867,11 @@
       <c r="N154" s="4">
         <v>0.3809523809523809</v>
       </c>
-    </row>
-    <row r="155" spans="1:14">
+      <c r="O154" s="4">
+        <v>0.5769230769230769</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15">
       <c r="A155" s="11" t="s">
         <v>41</v>
       </c>
@@ -7491,8 +7914,11 @@
       <c r="N155" s="4">
         <v>0.09174311926605504</v>
       </c>
-    </row>
-    <row r="156" spans="1:14">
+      <c r="O155" s="4">
+        <v>0.7407407407407407</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15">
       <c r="A156" s="12" t="s">
         <v>42</v>
       </c>
@@ -7535,8 +7961,11 @@
       <c r="N156" s="4">
         <v>0.5483870967741935</v>
       </c>
-    </row>
-    <row r="157" spans="1:14">
+      <c r="O156" s="4">
+        <v>1.12540192926045</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15">
       <c r="A157" s="12" t="s">
         <v>43</v>
       </c>
@@ -7579,8 +8008,11 @@
       <c r="N157" s="4">
         <v>0.881057268722467</v>
       </c>
-    </row>
-    <row r="158" spans="1:14">
+      <c r="O157" s="4">
+        <v>0.8260869565217391</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15">
       <c r="A158" s="13" t="s">
         <v>44</v>
       </c>
@@ -7623,8 +8055,11 @@
       <c r="N158" s="4">
         <v>0.5555555555555556</v>
       </c>
-    </row>
-    <row r="159" spans="1:14">
+      <c r="O158" s="4">
+        <v>0.2247191011235955</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15">
       <c r="A159" s="13" t="s">
         <v>45</v>
       </c>
@@ -7667,8 +8102,11 @@
       <c r="N159" s="4">
         <v>0.1923076923076923</v>
       </c>
-    </row>
-    <row r="160" spans="1:14">
+      <c r="O159" s="4">
+        <v>0.3921568627450981</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15">
       <c r="A160" s="6" t="s">
         <v>31</v>
       </c>
@@ -7709,6 +8147,9 @@
         <v>0</v>
       </c>
       <c r="N160" s="4">
+        <v>0</v>
+      </c>
+      <c r="O160" s="4">
         <v>0</v>
       </c>
     </row>
@@ -7832,6 +8273,9 @@
       <c r="N163" s="4">
         <v>0.5585585585585585</v>
       </c>
+      <c r="O163" s="4">
+        <v>0.5901639344262295</v>
+      </c>
     </row>
     <row r="164" spans="1:25">
       <c r="A164" s="3" t="s">
@@ -7876,6 +8320,9 @@
       <c r="N164" s="4">
         <v>0.1923076923076923</v>
       </c>
+      <c r="O164" s="4">
+        <v>0.2018502943650126</v>
+      </c>
     </row>
     <row r="165" spans="1:25">
       <c r="A165" s="5" t="s">
@@ -7920,6 +8367,9 @@
       <c r="N165" s="4">
         <v>0.483005366726297</v>
       </c>
+      <c r="O165" s="4">
+        <v>0.4811372334609076</v>
+      </c>
     </row>
     <row r="166" spans="1:25">
       <c r="A166" s="5" t="s">
@@ -7964,6 +8414,9 @@
       <c r="N166" s="4">
         <v>0.5409219190968956</v>
       </c>
+      <c r="O166" s="4">
+        <v>0.5417212756662297</v>
+      </c>
     </row>
     <row r="167" spans="1:25">
       <c r="A167" s="6" t="s">
@@ -8008,6 +8461,9 @@
       <c r="N167" s="4">
         <v>1.066292528937215</v>
       </c>
+      <c r="O167" s="4">
+        <v>1.057068741893645</v>
+      </c>
     </row>
     <row r="168" spans="1:25">
       <c r="A168" s="6" t="s">
@@ -8052,6 +8508,9 @@
       <c r="N168" s="4">
         <v>1.120032115616219</v>
       </c>
+      <c r="O168" s="4">
+        <v>1.082474226804124</v>
+      </c>
     </row>
     <row r="169" spans="1:25">
       <c r="A169" s="7" t="s">
@@ -8096,6 +8555,9 @@
       <c r="N169" s="4">
         <v>0.7180851063829787</v>
       </c>
+      <c r="O169" s="4">
+        <v>0.7010475423045931</v>
+      </c>
     </row>
     <row r="170" spans="1:25">
       <c r="A170" s="7" t="s">
@@ -8140,6 +8602,9 @@
       <c r="N170" s="4">
         <v>0.8017334777898159</v>
       </c>
+      <c r="O170" s="4">
+        <v>0.7465618860510805</v>
+      </c>
     </row>
     <row r="171" spans="1:25">
       <c r="A171" s="8" t="s">
@@ -8184,6 +8649,9 @@
       <c r="N171" s="4">
         <v>0.3985507246376812</v>
       </c>
+      <c r="O171" s="4">
+        <v>0.3982300884955752</v>
+      </c>
     </row>
     <row r="172" spans="1:25">
       <c r="A172" s="8" t="s">
@@ -8228,6 +8696,9 @@
       <c r="N172" s="4">
         <v>0.5287356321839081</v>
       </c>
+      <c r="O172" s="4">
+        <v>0.2969247083775186</v>
+      </c>
     </row>
     <row r="173" spans="1:25">
       <c r="A173" s="9" t="s">
@@ -8272,6 +8743,9 @@
       <c r="N173" s="4">
         <v>1.065625</v>
       </c>
+      <c r="O173" s="4">
+        <v>1.034084344309648</v>
+      </c>
     </row>
     <row r="174" spans="1:25">
       <c r="A174" s="9" t="s">
@@ -8316,6 +8790,9 @@
       <c r="N174" s="4">
         <v>1.096096096096096</v>
       </c>
+      <c r="O174" s="4">
+        <v>1.111494649637556</v>
+      </c>
     </row>
     <row r="175" spans="1:25">
       <c r="A175" s="10" t="s">
@@ -8360,6 +8837,9 @@
       <c r="N175" s="4">
         <v>0.9481765834932822</v>
       </c>
+      <c r="O175" s="4">
+        <v>1.033145275035261</v>
+      </c>
     </row>
     <row r="176" spans="1:25">
       <c r="A176" s="10" t="s">
@@ -8404,8 +8884,11 @@
       <c r="N176" s="4">
         <v>0.9179307662388175</v>
       </c>
-    </row>
-    <row r="177" spans="1:14">
+      <c r="O176" s="4">
+        <v>0.7725476104922745</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15">
       <c r="A177" s="11" t="s">
         <v>40</v>
       </c>
@@ -8448,8 +8931,11 @@
       <c r="N177" s="4">
         <v>0.6741573033707865</v>
       </c>
-    </row>
-    <row r="178" spans="1:14">
+      <c r="O177" s="4">
+        <v>0.6655290102389079</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15">
       <c r="A178" s="11" t="s">
         <v>41</v>
       </c>
@@ -8492,8 +8978,11 @@
       <c r="N178" s="4">
         <v>0.3085824493731919</v>
       </c>
-    </row>
-    <row r="179" spans="1:14">
+      <c r="O178" s="4">
+        <v>0.3493449781659388</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15">
       <c r="A179" s="12" t="s">
         <v>42</v>
       </c>
@@ -8536,8 +9025,11 @@
       <c r="N179" s="4">
         <v>1.038500506585613</v>
       </c>
-    </row>
-    <row r="180" spans="1:14">
+      <c r="O179" s="4">
+        <v>1.044846208030054</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15">
       <c r="A180" s="12" t="s">
         <v>43</v>
       </c>
@@ -8580,8 +9072,11 @@
       <c r="N180" s="4">
         <v>0.7668606641561109</v>
       </c>
-    </row>
-    <row r="181" spans="1:14">
+      <c r="O180" s="4">
+        <v>0.7711837511900983</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15">
       <c r="A181" s="13" t="s">
         <v>44</v>
       </c>
@@ -8624,8 +9119,11 @@
       <c r="N181" s="4">
         <v>0.1173959445037353</v>
       </c>
-    </row>
-    <row r="182" spans="1:14">
+      <c r="O181" s="4">
+        <v>0.1267056530214425</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15">
       <c r="A182" s="13" t="s">
         <v>45</v>
       </c>
@@ -8668,8 +9166,11 @@
       <c r="N182" s="4">
         <v>0.09523809523809523</v>
       </c>
-    </row>
-    <row r="183" spans="1:14">
+      <c r="O182" s="4">
+        <v>0.1174743024963289</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15">
       <c r="A183" s="6" t="s">
         <v>31</v>
       </c>
@@ -8710,6 +9211,9 @@
         <v>1.857142857142857</v>
       </c>
       <c r="N183" s="4">
+        <v>1.857142857142857</v>
+      </c>
+      <c r="O183" s="4">
         <v>1.857142857142857</v>
       </c>
     </row>
@@ -8846,6 +9350,9 @@
       <c r="N2" s="4">
         <v>-5</v>
       </c>
+      <c r="O2" s="4">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="5" t="s">
@@ -8890,6 +9397,9 @@
       <c r="N3" s="4">
         <v>23</v>
       </c>
+      <c r="O3" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="6" t="s">
@@ -8934,6 +9444,9 @@
       <c r="N4" s="4">
         <v>47</v>
       </c>
+      <c r="O4" s="4">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="7" t="s">
@@ -8978,6 +9491,9 @@
       <c r="N5" s="4">
         <v>10</v>
       </c>
+      <c r="O5" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="8" t="s">
@@ -9022,6 +9538,9 @@
       <c r="N6" s="4">
         <v>2</v>
       </c>
+      <c r="O6" s="4">
+        <v>-14</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="9" t="s">
@@ -9066,6 +9585,9 @@
       <c r="N7" s="4">
         <v>74</v>
       </c>
+      <c r="O7" s="4">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="10" t="s">
@@ -9110,6 +9632,9 @@
       <c r="N8" s="4">
         <v>58</v>
       </c>
+      <c r="O8" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="11" t="s">
@@ -9154,6 +9679,9 @@
       <c r="N9" s="4">
         <v>25</v>
       </c>
+      <c r="O9" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="12" t="s">
@@ -9198,6 +9726,9 @@
       <c r="N10" s="4">
         <v>42</v>
       </c>
+      <c r="O10" s="4">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="13" t="s">
@@ -9242,6 +9773,9 @@
       <c r="N11" s="4">
         <v>9</v>
       </c>
+      <c r="O11" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
@@ -9363,6 +9897,9 @@
       <c r="N14" s="4">
         <v>9.9</v>
       </c>
+      <c r="O14" s="4">
+        <v>9.699999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="5" t="s">
@@ -9407,6 +9944,9 @@
       <c r="N15" s="4">
         <v>15.4</v>
       </c>
+      <c r="O15" s="4">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="6" t="s">
@@ -9451,6 +9991,9 @@
       <c r="N16" s="4">
         <v>23.7</v>
       </c>
+      <c r="O16" s="4">
+        <v>23.4</v>
+      </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="7" t="s">
@@ -9495,6 +10038,9 @@
       <c r="N17" s="4">
         <v>10.4</v>
       </c>
+      <c r="O17" s="4">
+        <v>10.3</v>
+      </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="8" t="s">
@@ -9539,6 +10085,9 @@
       <c r="N18" s="4">
         <v>7</v>
       </c>
+      <c r="O18" s="4">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="9" t="s">
@@ -9583,6 +10132,9 @@
       <c r="N19" s="4">
         <v>25.8</v>
       </c>
+      <c r="O19" s="4">
+        <v>25.9</v>
+      </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="10" t="s">
@@ -9627,6 +10179,9 @@
       <c r="N20" s="4">
         <v>22.6</v>
       </c>
+      <c r="O20" s="4">
+        <v>22.9</v>
+      </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="11" t="s">
@@ -9671,6 +10226,9 @@
       <c r="N21" s="4">
         <v>10.7</v>
       </c>
+      <c r="O21" s="4">
+        <v>11.2</v>
+      </c>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="12" t="s">
@@ -9715,6 +10273,9 @@
       <c r="N22" s="4">
         <v>29</v>
       </c>
+      <c r="O22" s="4">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="13" t="s">
@@ -9759,6 +10320,9 @@
       <c r="N23" s="4">
         <v>6.6</v>
       </c>
+      <c r="O23" s="4">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="1" t="s">
@@ -9880,6 +10444,9 @@
       <c r="N26" s="4">
         <v>125</v>
       </c>
+      <c r="O26" s="4">
+        <v>143</v>
+      </c>
     </row>
     <row r="27" spans="1:25">
       <c r="A27" s="5" t="s">
@@ -9924,6 +10491,9 @@
       <c r="N27" s="4">
         <v>275</v>
       </c>
+      <c r="O27" s="4">
+        <v>296</v>
+      </c>
     </row>
     <row r="28" spans="1:25">
       <c r="A28" s="6" t="s">
@@ -9968,6 +10538,9 @@
       <c r="N28" s="4">
         <v>733</v>
       </c>
+      <c r="O28" s="4">
+        <v>780</v>
+      </c>
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="7" t="s">
@@ -10012,6 +10585,9 @@
       <c r="N29" s="4">
         <v>195</v>
       </c>
+      <c r="O29" s="4">
+        <v>202</v>
+      </c>
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="8" t="s">
@@ -10056,6 +10632,9 @@
       <c r="N30" s="4">
         <v>87</v>
       </c>
+      <c r="O30" s="4">
+        <v>73</v>
+      </c>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="9" t="s">
@@ -10100,6 +10679,9 @@
       <c r="N31" s="4">
         <v>699</v>
       </c>
+      <c r="O31" s="4">
+        <v>766</v>
+      </c>
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="10" t="s">
@@ -10144,6 +10726,9 @@
       <c r="N32" s="4">
         <v>603</v>
       </c>
+      <c r="O32" s="4">
+        <v>628</v>
+      </c>
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="11" t="s">
@@ -10188,6 +10773,9 @@
       <c r="N33" s="4">
         <v>178</v>
       </c>
+      <c r="O33" s="4">
+        <v>195</v>
+      </c>
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="12" t="s">
@@ -10232,6 +10820,9 @@
       <c r="N34" s="4">
         <v>859</v>
       </c>
+      <c r="O34" s="4">
+        <v>928</v>
+      </c>
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="13" t="s">
@@ -10276,6 +10867,9 @@
       <c r="N35" s="4">
         <v>40</v>
       </c>
+      <c r="O35" s="4">
+        <v>45</v>
+      </c>
     </row>
     <row r="37" spans="1:25">
       <c r="A37" s="1" t="s">
@@ -10397,6 +10991,9 @@
       <c r="N38" s="4">
         <v>112.1</v>
       </c>
+      <c r="O38" s="4">
+        <v>121.8</v>
+      </c>
     </row>
     <row r="39" spans="1:25">
       <c r="A39" s="5" t="s">
@@ -10441,6 +11038,9 @@
       <c r="N39" s="4">
         <v>192.6</v>
       </c>
+      <c r="O39" s="4">
+        <v>208.1</v>
+      </c>
     </row>
     <row r="40" spans="1:25">
       <c r="A40" s="6" t="s">
@@ -10485,6 +11085,9 @@
       <c r="N40" s="4">
         <v>281.4</v>
       </c>
+      <c r="O40" s="4">
+        <v>304.8</v>
+      </c>
     </row>
     <row r="41" spans="1:25">
       <c r="A41" s="7" t="s">
@@ -10529,6 +11132,9 @@
       <c r="N41" s="4">
         <v>108.4</v>
       </c>
+      <c r="O41" s="4">
+        <v>118.7</v>
+      </c>
     </row>
     <row r="42" spans="1:25">
       <c r="A42" s="8" t="s">
@@ -10573,6 +11179,9 @@
       <c r="N42" s="4">
         <v>85.59999999999999</v>
       </c>
+      <c r="O42" s="4">
+        <v>92.5</v>
+      </c>
     </row>
     <row r="43" spans="1:25">
       <c r="A43" s="9" t="s">
@@ -10617,6 +11226,9 @@
       <c r="N43" s="4">
         <v>319.1</v>
       </c>
+      <c r="O43" s="4">
+        <v>344.9999999999999</v>
+      </c>
     </row>
     <row r="44" spans="1:25">
       <c r="A44" s="10" t="s">
@@ -10661,6 +11273,9 @@
       <c r="N44" s="4">
         <v>272.2</v>
       </c>
+      <c r="O44" s="4">
+        <v>295.1</v>
+      </c>
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="11" t="s">
@@ -10705,6 +11320,9 @@
       <c r="N45" s="4">
         <v>118.4</v>
       </c>
+      <c r="O45" s="4">
+        <v>129.6</v>
+      </c>
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="12" t="s">
@@ -10749,6 +11367,9 @@
       <c r="N46" s="4">
         <v>371.1999999999999</v>
       </c>
+      <c r="O46" s="4">
+        <v>400.1999999999999</v>
+      </c>
     </row>
     <row r="47" spans="1:25">
       <c r="A47" s="13" t="s">
@@ -10793,6 +11414,9 @@
       <c r="N47" s="4">
         <v>82.39999999999998</v>
       </c>
+      <c r="O47" s="4">
+        <v>88.89999999999998</v>
+      </c>
     </row>
     <row r="49" spans="1:25">
       <c r="A49" s="1" t="s">
@@ -10914,6 +11538,9 @@
       <c r="N50" s="4">
         <v>9.615384615384615</v>
       </c>
+      <c r="O50" s="4">
+        <v>10.21428571428571</v>
+      </c>
     </row>
     <row r="51" spans="1:25">
       <c r="A51" s="5" t="s">
@@ -10958,6 +11585,9 @@
       <c r="N51" s="4">
         <v>21.15384615384615</v>
       </c>
+      <c r="O51" s="4">
+        <v>21.14285714285714</v>
+      </c>
     </row>
     <row r="52" spans="1:25">
       <c r="A52" s="6" t="s">
@@ -11002,6 +11632,9 @@
       <c r="N52" s="4">
         <v>56.38461538461539</v>
       </c>
+      <c r="O52" s="4">
+        <v>55.71428571428572</v>
+      </c>
     </row>
     <row r="53" spans="1:25">
       <c r="A53" s="7" t="s">
@@ -11046,6 +11679,9 @@
       <c r="N53" s="4">
         <v>15</v>
       </c>
+      <c r="O53" s="4">
+        <v>14.42857142857143</v>
+      </c>
     </row>
     <row r="54" spans="1:25">
       <c r="A54" s="8" t="s">
@@ -11090,6 +11726,9 @@
       <c r="N54" s="4">
         <v>6.692307692307693</v>
       </c>
+      <c r="O54" s="4">
+        <v>5.214285714285714</v>
+      </c>
     </row>
     <row r="55" spans="1:25">
       <c r="A55" s="9" t="s">
@@ -11134,6 +11773,9 @@
       <c r="N55" s="4">
         <v>53.76923076923077</v>
       </c>
+      <c r="O55" s="4">
+        <v>54.71428571428572</v>
+      </c>
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="10" t="s">
@@ -11178,6 +11820,9 @@
       <c r="N56" s="4">
         <v>46.38461538461539</v>
       </c>
+      <c r="O56" s="4">
+        <v>44.85714285714285</v>
+      </c>
     </row>
     <row r="57" spans="1:25">
       <c r="A57" s="11" t="s">
@@ -11222,6 +11867,9 @@
       <c r="N57" s="4">
         <v>13.69230769230769</v>
       </c>
+      <c r="O57" s="4">
+        <v>13.92857142857143</v>
+      </c>
     </row>
     <row r="58" spans="1:25">
       <c r="A58" s="12" t="s">
@@ -11266,6 +11914,9 @@
       <c r="N58" s="4">
         <v>66.07692307692308</v>
       </c>
+      <c r="O58" s="4">
+        <v>66.28571428571429</v>
+      </c>
     </row>
     <row r="59" spans="1:25">
       <c r="A59" s="13" t="s">
@@ -11310,6 +11961,9 @@
       <c r="N59" s="4">
         <v>3.076923076923077</v>
       </c>
+      <c r="O59" s="4">
+        <v>3.214285714285714</v>
+      </c>
     </row>
     <row r="61" spans="1:25">
       <c r="A61" s="1" t="s">
@@ -11431,6 +12085,9 @@
       <c r="N62" s="4">
         <v>8.623076923076921</v>
       </c>
+      <c r="O62" s="4">
+        <v>8.699999999999999</v>
+      </c>
     </row>
     <row r="63" spans="1:25">
       <c r="A63" s="5" t="s">
@@ -11475,6 +12132,9 @@
       <c r="N63" s="4">
         <v>14.81538461538461</v>
       </c>
+      <c r="O63" s="4">
+        <v>14.86428571428571</v>
+      </c>
     </row>
     <row r="64" spans="1:25">
       <c r="A64" s="6" t="s">
@@ -11519,6 +12179,9 @@
       <c r="N64" s="4">
         <v>21.64615384615384</v>
       </c>
+      <c r="O64" s="4">
+        <v>21.77142857142857</v>
+      </c>
     </row>
     <row r="65" spans="1:25">
       <c r="A65" s="7" t="s">
@@ -11563,6 +12226,9 @@
       <c r="N65" s="4">
         <v>8.338461538461541</v>
       </c>
+      <c r="O65" s="4">
+        <v>8.47857142857143</v>
+      </c>
     </row>
     <row r="66" spans="1:25">
       <c r="A66" s="8" t="s">
@@ -11607,6 +12273,9 @@
       <c r="N66" s="4">
         <v>6.584615384615384</v>
       </c>
+      <c r="O66" s="4">
+        <v>6.607142857142857</v>
+      </c>
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="9" t="s">
@@ -11651,6 +12320,9 @@
       <c r="N67" s="4">
         <v>24.54615384615384</v>
       </c>
+      <c r="O67" s="4">
+        <v>24.64285714285714</v>
+      </c>
     </row>
     <row r="68" spans="1:25">
       <c r="A68" s="10" t="s">
@@ -11695,6 +12367,9 @@
       <c r="N68" s="4">
         <v>20.93846153846154</v>
       </c>
+      <c r="O68" s="4">
+        <v>21.07857142857143</v>
+      </c>
     </row>
     <row r="69" spans="1:25">
       <c r="A69" s="11" t="s">
@@ -11739,6 +12414,9 @@
       <c r="N69" s="4">
         <v>9.107692307692307</v>
       </c>
+      <c r="O69" s="4">
+        <v>9.257142857142856</v>
+      </c>
     </row>
     <row r="70" spans="1:25">
       <c r="A70" s="12" t="s">
@@ -11783,6 +12461,9 @@
       <c r="N70" s="4">
         <v>28.55384615384615</v>
       </c>
+      <c r="O70" s="4">
+        <v>28.58571428571428</v>
+      </c>
     </row>
     <row r="71" spans="1:25">
       <c r="A71" s="13" t="s">
@@ -11827,6 +12508,9 @@
       <c r="N71" s="4">
         <v>6.338461538461536</v>
       </c>
+      <c r="O71" s="4">
+        <v>6.349999999999999</v>
+      </c>
     </row>
     <row r="73" spans="1:25">
       <c r="A73" s="1" t="s">
@@ -11948,6 +12632,9 @@
       <c r="N74" s="4">
         <v>-0.5050505050505051</v>
       </c>
+      <c r="O74" s="4">
+        <v>1.855670103092784</v>
+      </c>
     </row>
     <row r="75" spans="1:25">
       <c r="A75" s="5" t="s">
@@ -11992,6 +12679,9 @@
       <c r="N75" s="4">
         <v>1.493506493506493</v>
       </c>
+      <c r="O75" s="4">
+        <v>1.354838709677419</v>
+      </c>
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="6" t="s">
@@ -12036,6 +12726,9 @@
       <c r="N76" s="4">
         <v>1.983122362869198</v>
       </c>
+      <c r="O76" s="4">
+        <v>2.008547008547009</v>
+      </c>
     </row>
     <row r="77" spans="1:25">
       <c r="A77" s="7" t="s">
@@ -12080,6 +12773,9 @@
       <c r="N77" s="4">
         <v>0.9615384615384615</v>
       </c>
+      <c r="O77" s="4">
+        <v>0.6796116504854368</v>
+      </c>
     </row>
     <row r="78" spans="1:25">
       <c r="A78" s="8" t="s">
@@ -12124,6 +12820,9 @@
       <c r="N78" s="4">
         <v>0.2857142857142857</v>
       </c>
+      <c r="O78" s="4">
+        <v>-2.028985507246376</v>
+      </c>
     </row>
     <row r="79" spans="1:25">
       <c r="A79" s="9" t="s">
@@ -12168,6 +12867,9 @@
       <c r="N79" s="4">
         <v>2.868217054263566</v>
       </c>
+      <c r="O79" s="4">
+        <v>2.586872586872587</v>
+      </c>
     </row>
     <row r="80" spans="1:25">
       <c r="A80" s="10" t="s">
@@ -12212,6 +12914,9 @@
       <c r="N80" s="4">
         <v>2.566371681415929</v>
       </c>
+      <c r="O80" s="4">
+        <v>1.091703056768559</v>
+      </c>
     </row>
     <row r="81" spans="1:25">
       <c r="A81" s="11" t="s">
@@ -12256,6 +12961,9 @@
       <c r="N81" s="4">
         <v>2.336448598130841</v>
       </c>
+      <c r="O81" s="4">
+        <v>1.517857142857143</v>
+      </c>
     </row>
     <row r="82" spans="1:25">
       <c r="A82" s="12" t="s">
@@ -12300,6 +13008,9 @@
       <c r="N82" s="4">
         <v>1.448275862068966</v>
       </c>
+      <c r="O82" s="4">
+        <v>2.379310344827586</v>
+      </c>
     </row>
     <row r="83" spans="1:25">
       <c r="A83" s="13" t="s">
@@ -12344,6 +13055,9 @@
       <c r="N83" s="4">
         <v>1.363636363636364</v>
       </c>
+      <c r="O83" s="4">
+        <v>0.7692307692307693</v>
+      </c>
     </row>
     <row r="85" spans="1:25">
       <c r="A85" s="1" t="s">
@@ -12465,6 +13179,9 @@
       <c r="N86" s="4">
         <v>1.115075825156111</v>
       </c>
+      <c r="O86" s="4">
+        <v>1.174055829228243</v>
+      </c>
     </row>
     <row r="87" spans="1:25">
       <c r="A87" s="5" t="s">
@@ -12509,6 +13226,9 @@
       <c r="N87" s="4">
         <v>1.427829698857736</v>
       </c>
+      <c r="O87" s="4">
+        <v>1.42239308024988</v>
+      </c>
     </row>
     <row r="88" spans="1:25">
       <c r="A88" s="6" t="s">
@@ -12553,6 +13273,9 @@
       <c r="N88" s="4">
         <v>2.604832977967307</v>
       </c>
+      <c r="O88" s="4">
+        <v>2.559055118110236</v>
+      </c>
     </row>
     <row r="89" spans="1:25">
       <c r="A89" s="7" t="s">
@@ -12597,6 +13320,9 @@
       <c r="N89" s="4">
         <v>1.798892988929889</v>
       </c>
+      <c r="O89" s="4">
+        <v>1.701769165964617</v>
+      </c>
     </row>
     <row r="90" spans="1:25">
       <c r="A90" s="8" t="s">
@@ -12641,6 +13367,9 @@
       <c r="N90" s="4">
         <v>1.016355140186916</v>
       </c>
+      <c r="O90" s="4">
+        <v>0.7891891891891892</v>
+      </c>
     </row>
     <row r="91" spans="1:25">
       <c r="A91" s="9" t="s">
@@ -12685,6 +13414,9 @@
       <c r="N91" s="4">
         <v>2.190535882168599</v>
       </c>
+      <c r="O91" s="4">
+        <v>2.220289855072464</v>
+      </c>
     </row>
     <row r="92" spans="1:25">
       <c r="A92" s="10" t="s">
@@ -12729,6 +13461,9 @@
       <c r="N92" s="4">
         <v>2.215282880235121</v>
       </c>
+      <c r="O92" s="4">
+        <v>2.128092172145035</v>
+      </c>
     </row>
     <row r="93" spans="1:25">
       <c r="A93" s="11" t="s">
@@ -12773,6 +13508,9 @@
       <c r="N93" s="4">
         <v>1.503378378378378</v>
       </c>
+      <c r="O93" s="4">
+        <v>1.50462962962963</v>
+      </c>
     </row>
     <row r="94" spans="1:25">
       <c r="A94" s="12" t="s">
@@ -12817,6 +13555,9 @@
       <c r="N94" s="4">
         <v>2.314116379310345</v>
       </c>
+      <c r="O94" s="4">
+        <v>2.318840579710145</v>
+      </c>
     </row>
     <row r="95" spans="1:25">
       <c r="A95" s="13" t="s">
@@ -12860,6 +13601,9 @@
       </c>
       <c r="N95" s="4">
         <v>0.4854368932038834</v>
+      </c>
+      <c r="O95" s="4">
+        <v>0.5061867266591675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>